<commit_message>
Revised based on comments
</commit_message>
<xml_diff>
--- a/src/sst_details.xlsx
+++ b/src/sst_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://prevalonenergy-my.sharepoint.com/personal/himanshu_prevalonenergy_com/Documents/I drive/Knowledge Scraper/deploy/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="11_F25DC773A252ABDACC1048B2119E5C9C5BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4402C44C-F082-48DE-8A9A-03E65EEAFEA5}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="11_F25DC773A252ABDACC1048B2119E5C9C5BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC25768B-188F-4431-B58F-23E5ABC7E812}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -384,7 +384,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,7 +406,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -414,7 +414,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>1600</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -422,8 +422,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <f>$B$3*(1-0.01)^5</f>
-        <v>1521.58407984</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -431,8 +430,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <f>$B$3*(1-0.01)^10</f>
-        <v>1447.0113200140868</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -441,7 +439,7 @@
       </c>
       <c r="B6" s="1">
         <f>$B$3*(1-0.01)^15</f>
-        <v>1376.0933674260614</v>
+        <v>860.05835464128836</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -450,7 +448,7 @@
       </c>
       <c r="B7" s="1">
         <f>$B$3*(1-0.01)^20</f>
-        <v>1308.6511001555691</v>
+        <v>817.90693759723069</v>
       </c>
     </row>
   </sheetData>

</xml_diff>